<commit_message>
Updated NFL penalties to include 2019, added wins & losses data
</commit_message>
<xml_diff>
--- a/nfl-penalties/data/by_team_group.xlsx
+++ b/nfl-penalties/data/by_team_group.xlsx
@@ -16,6 +16,7 @@
     <sheet name="2016" sheetId="8" state="visible" r:id="rId8"/>
     <sheet name="2017" sheetId="9" state="visible" r:id="rId9"/>
     <sheet name="2018" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="2019" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
 </workbook>
 </file>
@@ -101,7 +102,7 @@
     <t xml:space="preserve">Kansas City</t>
   </si>
   <si>
-    <t xml:space="preserve">Oakland</t>
+    <t xml:space="preserve">Las Vegas</t>
   </si>
   <si>
     <t xml:space="preserve">LA Chargers</t>
@@ -485,7 +486,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -1791,7 +1792,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -3083,6 +3084,1312 @@
       </c>
       <c r="L34" t="n">
         <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="n">
+        <v>124</v>
+      </c>
+      <c r="C2" t="n">
+        <v>991</v>
+      </c>
+      <c r="D2" t="n">
+        <v>64</v>
+      </c>
+      <c r="E2" t="n">
+        <v>509</v>
+      </c>
+      <c r="F2" t="n">
+        <v>50</v>
+      </c>
+      <c r="G2" t="n">
+        <v>394</v>
+      </c>
+      <c r="H2" t="n">
+        <v>10</v>
+      </c>
+      <c r="I2" t="n">
+        <v>88</v>
+      </c>
+      <c r="J2" t="n">
+        <v>31</v>
+      </c>
+      <c r="K2" t="n">
+        <v>16</v>
+      </c>
+      <c r="L2" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" t="n">
+        <v>92</v>
+      </c>
+      <c r="C3" t="n">
+        <v>769</v>
+      </c>
+      <c r="D3" t="n">
+        <v>33</v>
+      </c>
+      <c r="E3" t="n">
+        <v>250</v>
+      </c>
+      <c r="F3" t="n">
+        <v>44</v>
+      </c>
+      <c r="G3" t="n">
+        <v>416</v>
+      </c>
+      <c r="H3" t="n">
+        <v>15</v>
+      </c>
+      <c r="I3" t="n">
+        <v>103</v>
+      </c>
+      <c r="J3" t="n">
+        <v>14</v>
+      </c>
+      <c r="K3" t="n">
+        <v>6</v>
+      </c>
+      <c r="L3" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="n">
+        <v>97</v>
+      </c>
+      <c r="C4" t="n">
+        <v>856</v>
+      </c>
+      <c r="D4" t="n">
+        <v>43</v>
+      </c>
+      <c r="E4" t="n">
+        <v>362</v>
+      </c>
+      <c r="F4" t="n">
+        <v>41</v>
+      </c>
+      <c r="G4" t="n">
+        <v>391</v>
+      </c>
+      <c r="H4" t="n">
+        <v>13</v>
+      </c>
+      <c r="I4" t="n">
+        <v>103</v>
+      </c>
+      <c r="J4" t="n">
+        <v>13</v>
+      </c>
+      <c r="K4" t="n">
+        <v>4</v>
+      </c>
+      <c r="L4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="n">
+        <v>115</v>
+      </c>
+      <c r="C5" t="n">
+        <v>1105</v>
+      </c>
+      <c r="D5" t="n">
+        <v>50</v>
+      </c>
+      <c r="E5" t="n">
+        <v>406</v>
+      </c>
+      <c r="F5" t="n">
+        <v>48</v>
+      </c>
+      <c r="G5" t="n">
+        <v>533</v>
+      </c>
+      <c r="H5" t="n">
+        <v>17</v>
+      </c>
+      <c r="I5" t="n">
+        <v>166</v>
+      </c>
+      <c r="J5" t="n">
+        <v>14</v>
+      </c>
+      <c r="K5" t="n">
+        <v>9</v>
+      </c>
+      <c r="L5" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" t="n">
+        <v>116</v>
+      </c>
+      <c r="C6" t="n">
+        <v>923</v>
+      </c>
+      <c r="D6" t="n">
+        <v>46</v>
+      </c>
+      <c r="E6" t="n">
+        <v>328</v>
+      </c>
+      <c r="F6" t="n">
+        <v>49</v>
+      </c>
+      <c r="G6" t="n">
+        <v>436</v>
+      </c>
+      <c r="H6" t="n">
+        <v>21</v>
+      </c>
+      <c r="I6" t="n">
+        <v>159</v>
+      </c>
+      <c r="J6" t="n">
+        <v>24</v>
+      </c>
+      <c r="K6" t="n">
+        <v>6</v>
+      </c>
+      <c r="L6" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B7" t="n">
+        <v>93</v>
+      </c>
+      <c r="C7" t="n">
+        <v>761</v>
+      </c>
+      <c r="D7" t="n">
+        <v>49</v>
+      </c>
+      <c r="E7" t="n">
+        <v>360</v>
+      </c>
+      <c r="F7" t="n">
+        <v>28</v>
+      </c>
+      <c r="G7" t="n">
+        <v>256</v>
+      </c>
+      <c r="H7" t="n">
+        <v>16</v>
+      </c>
+      <c r="I7" t="n">
+        <v>145</v>
+      </c>
+      <c r="J7" t="n">
+        <v>28</v>
+      </c>
+      <c r="K7" t="n">
+        <v>6</v>
+      </c>
+      <c r="L7" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="n">
+        <v>122</v>
+      </c>
+      <c r="C8" t="n">
+        <v>1106</v>
+      </c>
+      <c r="D8" t="n">
+        <v>60</v>
+      </c>
+      <c r="E8" t="n">
+        <v>457</v>
+      </c>
+      <c r="F8" t="n">
+        <v>48</v>
+      </c>
+      <c r="G8" t="n">
+        <v>524</v>
+      </c>
+      <c r="H8" t="n">
+        <v>13</v>
+      </c>
+      <c r="I8" t="n">
+        <v>110</v>
+      </c>
+      <c r="J8" t="n">
+        <v>30</v>
+      </c>
+      <c r="K8" t="n">
+        <v>8</v>
+      </c>
+      <c r="L8" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" t="n">
+        <v>111</v>
+      </c>
+      <c r="C9" t="n">
+        <v>887</v>
+      </c>
+      <c r="D9" t="n">
+        <v>53</v>
+      </c>
+      <c r="E9" t="n">
+        <v>387</v>
+      </c>
+      <c r="F9" t="n">
+        <v>41</v>
+      </c>
+      <c r="G9" t="n">
+        <v>375</v>
+      </c>
+      <c r="H9" t="n">
+        <v>17</v>
+      </c>
+      <c r="I9" t="n">
+        <v>125</v>
+      </c>
+      <c r="J9" t="n">
+        <v>25</v>
+      </c>
+      <c r="K9" t="n">
+        <v>13</v>
+      </c>
+      <c r="L9" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="n">
+        <v>122</v>
+      </c>
+      <c r="C10" t="n">
+        <v>999</v>
+      </c>
+      <c r="D10" t="n">
+        <v>61</v>
+      </c>
+      <c r="E10" t="n">
+        <v>406</v>
+      </c>
+      <c r="F10" t="n">
+        <v>45</v>
+      </c>
+      <c r="G10" t="n">
+        <v>466</v>
+      </c>
+      <c r="H10" t="n">
+        <v>16</v>
+      </c>
+      <c r="I10" t="n">
+        <v>127</v>
+      </c>
+      <c r="J10" t="n">
+        <v>39</v>
+      </c>
+      <c r="K10" t="n">
+        <v>10</v>
+      </c>
+      <c r="L10" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="n">
+        <v>79</v>
+      </c>
+      <c r="C11" t="n">
+        <v>670</v>
+      </c>
+      <c r="D11" t="n">
+        <v>40</v>
+      </c>
+      <c r="E11" t="n">
+        <v>308</v>
+      </c>
+      <c r="F11" t="n">
+        <v>26</v>
+      </c>
+      <c r="G11" t="n">
+        <v>253</v>
+      </c>
+      <c r="H11" t="n">
+        <v>13</v>
+      </c>
+      <c r="I11" t="n">
+        <v>109</v>
+      </c>
+      <c r="J11" t="n">
+        <v>14</v>
+      </c>
+      <c r="K11" t="n">
+        <v>4</v>
+      </c>
+      <c r="L11" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>22</v>
+      </c>
+      <c r="B12" t="n">
+        <v>132</v>
+      </c>
+      <c r="C12" t="n">
+        <v>1169</v>
+      </c>
+      <c r="D12" t="n">
+        <v>62</v>
+      </c>
+      <c r="E12" t="n">
+        <v>504</v>
+      </c>
+      <c r="F12" t="n">
+        <v>46</v>
+      </c>
+      <c r="G12" t="n">
+        <v>448</v>
+      </c>
+      <c r="H12" t="n">
+        <v>24</v>
+      </c>
+      <c r="I12" t="n">
+        <v>217</v>
+      </c>
+      <c r="J12" t="n">
+        <v>18</v>
+      </c>
+      <c r="K12" t="n">
+        <v>13</v>
+      </c>
+      <c r="L12" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="n">
+        <v>117</v>
+      </c>
+      <c r="C13" t="n">
+        <v>1062</v>
+      </c>
+      <c r="D13" t="n">
+        <v>62</v>
+      </c>
+      <c r="E13" t="n">
+        <v>465</v>
+      </c>
+      <c r="F13" t="n">
+        <v>39</v>
+      </c>
+      <c r="G13" t="n">
+        <v>470</v>
+      </c>
+      <c r="H13" t="n">
+        <v>16</v>
+      </c>
+      <c r="I13" t="n">
+        <v>127</v>
+      </c>
+      <c r="J13" t="n">
+        <v>31</v>
+      </c>
+      <c r="K13" t="n">
+        <v>6</v>
+      </c>
+      <c r="L13" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>24</v>
+      </c>
+      <c r="B14" t="n">
+        <v>110</v>
+      </c>
+      <c r="C14" t="n">
+        <v>912</v>
+      </c>
+      <c r="D14" t="n">
+        <v>53</v>
+      </c>
+      <c r="E14" t="n">
+        <v>431</v>
+      </c>
+      <c r="F14" t="n">
+        <v>42</v>
+      </c>
+      <c r="G14" t="n">
+        <v>365</v>
+      </c>
+      <c r="H14" t="n">
+        <v>15</v>
+      </c>
+      <c r="I14" t="n">
+        <v>116</v>
+      </c>
+      <c r="J14" t="n">
+        <v>20</v>
+      </c>
+      <c r="K14" t="n">
+        <v>8</v>
+      </c>
+      <c r="L14" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" t="n">
+        <v>124</v>
+      </c>
+      <c r="C15" t="n">
+        <v>1151</v>
+      </c>
+      <c r="D15" t="n">
+        <v>47</v>
+      </c>
+      <c r="E15" t="n">
+        <v>419</v>
+      </c>
+      <c r="F15" t="n">
+        <v>54</v>
+      </c>
+      <c r="G15" t="n">
+        <v>524</v>
+      </c>
+      <c r="H15" t="n">
+        <v>23</v>
+      </c>
+      <c r="I15" t="n">
+        <v>208</v>
+      </c>
+      <c r="J15" t="n">
+        <v>15</v>
+      </c>
+      <c r="K15" t="n">
+        <v>11</v>
+      </c>
+      <c r="L15" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B16" t="n">
+        <v>128</v>
+      </c>
+      <c r="C16" t="n">
+        <v>1138</v>
+      </c>
+      <c r="D16" t="n">
+        <v>42</v>
+      </c>
+      <c r="E16" t="n">
+        <v>322</v>
+      </c>
+      <c r="F16" t="n">
+        <v>68</v>
+      </c>
+      <c r="G16" t="n">
+        <v>634</v>
+      </c>
+      <c r="H16" t="n">
+        <v>18</v>
+      </c>
+      <c r="I16" t="n">
+        <v>182</v>
+      </c>
+      <c r="J16" t="n">
+        <v>19</v>
+      </c>
+      <c r="K16" t="n">
+        <v>21</v>
+      </c>
+      <c r="L16" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" t="n">
+        <v>103</v>
+      </c>
+      <c r="C17" t="n">
+        <v>872</v>
+      </c>
+      <c r="D17" t="n">
+        <v>51</v>
+      </c>
+      <c r="E17" t="n">
+        <v>415</v>
+      </c>
+      <c r="F17" t="n">
+        <v>37</v>
+      </c>
+      <c r="G17" t="n">
+        <v>335</v>
+      </c>
+      <c r="H17" t="n">
+        <v>15</v>
+      </c>
+      <c r="I17" t="n">
+        <v>122</v>
+      </c>
+      <c r="J17" t="n">
+        <v>22</v>
+      </c>
+      <c r="K17" t="n">
+        <v>10</v>
+      </c>
+      <c r="L17" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>28</v>
+      </c>
+      <c r="B18" t="n">
+        <v>109</v>
+      </c>
+      <c r="C18" t="n">
+        <v>1008</v>
+      </c>
+      <c r="D18" t="n">
+        <v>45</v>
+      </c>
+      <c r="E18" t="n">
+        <v>407</v>
+      </c>
+      <c r="F18" t="n">
+        <v>49</v>
+      </c>
+      <c r="G18" t="n">
+        <v>479</v>
+      </c>
+      <c r="H18" t="n">
+        <v>15</v>
+      </c>
+      <c r="I18" t="n">
+        <v>122</v>
+      </c>
+      <c r="J18" t="n">
+        <v>12</v>
+      </c>
+      <c r="K18" t="n">
+        <v>18</v>
+      </c>
+      <c r="L18" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B19" t="n">
+        <v>90</v>
+      </c>
+      <c r="C19" t="n">
+        <v>784</v>
+      </c>
+      <c r="D19" t="n">
+        <v>37</v>
+      </c>
+      <c r="E19" t="n">
+        <v>295</v>
+      </c>
+      <c r="F19" t="n">
+        <v>39</v>
+      </c>
+      <c r="G19" t="n">
+        <v>370</v>
+      </c>
+      <c r="H19" t="n">
+        <v>14</v>
+      </c>
+      <c r="I19" t="n">
+        <v>119</v>
+      </c>
+      <c r="J19" t="n">
+        <v>13</v>
+      </c>
+      <c r="K19" t="n">
+        <v>8</v>
+      </c>
+      <c r="L19" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="n">
+        <v>107</v>
+      </c>
+      <c r="C20" t="n">
+        <v>881</v>
+      </c>
+      <c r="D20" t="n">
+        <v>53</v>
+      </c>
+      <c r="E20" t="n">
+        <v>408</v>
+      </c>
+      <c r="F20" t="n">
+        <v>43</v>
+      </c>
+      <c r="G20" t="n">
+        <v>365</v>
+      </c>
+      <c r="H20" t="n">
+        <v>11</v>
+      </c>
+      <c r="I20" t="n">
+        <v>108</v>
+      </c>
+      <c r="J20" t="n">
+        <v>23</v>
+      </c>
+      <c r="K20" t="n">
+        <v>12</v>
+      </c>
+      <c r="L20" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" t="n">
+        <v>106</v>
+      </c>
+      <c r="C21" t="n">
+        <v>835</v>
+      </c>
+      <c r="D21" t="n">
+        <v>51</v>
+      </c>
+      <c r="E21" t="n">
+        <v>365</v>
+      </c>
+      <c r="F21" t="n">
+        <v>40</v>
+      </c>
+      <c r="G21" t="n">
+        <v>358</v>
+      </c>
+      <c r="H21" t="n">
+        <v>15</v>
+      </c>
+      <c r="I21" t="n">
+        <v>112</v>
+      </c>
+      <c r="J21" t="n">
+        <v>26</v>
+      </c>
+      <c r="K21" t="n">
+        <v>6</v>
+      </c>
+      <c r="L21" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>32</v>
+      </c>
+      <c r="B22" t="n">
+        <v>103</v>
+      </c>
+      <c r="C22" t="n">
+        <v>855</v>
+      </c>
+      <c r="D22" t="n">
+        <v>47</v>
+      </c>
+      <c r="E22" t="n">
+        <v>383</v>
+      </c>
+      <c r="F22" t="n">
+        <v>38</v>
+      </c>
+      <c r="G22" t="n">
+        <v>323</v>
+      </c>
+      <c r="H22" t="n">
+        <v>18</v>
+      </c>
+      <c r="I22" t="n">
+        <v>149</v>
+      </c>
+      <c r="J22" t="n">
+        <v>19</v>
+      </c>
+      <c r="K22" t="n">
+        <v>12</v>
+      </c>
+      <c r="L22" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>33</v>
+      </c>
+      <c r="B23" t="n">
+        <v>113</v>
+      </c>
+      <c r="C23" t="n">
+        <v>937</v>
+      </c>
+      <c r="D23" t="n">
+        <v>52</v>
+      </c>
+      <c r="E23" t="n">
+        <v>412</v>
+      </c>
+      <c r="F23" t="n">
+        <v>42</v>
+      </c>
+      <c r="G23" t="n">
+        <v>346</v>
+      </c>
+      <c r="H23" t="n">
+        <v>19</v>
+      </c>
+      <c r="I23" t="n">
+        <v>179</v>
+      </c>
+      <c r="J23" t="n">
+        <v>22</v>
+      </c>
+      <c r="K23" t="n">
+        <v>5</v>
+      </c>
+      <c r="L23" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>34</v>
+      </c>
+      <c r="B24" t="n">
+        <v>110</v>
+      </c>
+      <c r="C24" t="n">
+        <v>850</v>
+      </c>
+      <c r="D24" t="n">
+        <v>65</v>
+      </c>
+      <c r="E24" t="n">
+        <v>487</v>
+      </c>
+      <c r="F24" t="n">
+        <v>32</v>
+      </c>
+      <c r="G24" t="n">
+        <v>268</v>
+      </c>
+      <c r="H24" t="n">
+        <v>13</v>
+      </c>
+      <c r="I24" t="n">
+        <v>95</v>
+      </c>
+      <c r="J24" t="n">
+        <v>32</v>
+      </c>
+      <c r="K24" t="n">
+        <v>9</v>
+      </c>
+      <c r="L24" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>35</v>
+      </c>
+      <c r="B25" t="n">
+        <v>101</v>
+      </c>
+      <c r="C25" t="n">
+        <v>950</v>
+      </c>
+      <c r="D25" t="n">
+        <v>55</v>
+      </c>
+      <c r="E25" t="n">
+        <v>486</v>
+      </c>
+      <c r="F25" t="n">
+        <v>35</v>
+      </c>
+      <c r="G25" t="n">
+        <v>378</v>
+      </c>
+      <c r="H25" t="n">
+        <v>11</v>
+      </c>
+      <c r="I25" t="n">
+        <v>86</v>
+      </c>
+      <c r="J25" t="n">
+        <v>17</v>
+      </c>
+      <c r="K25" t="n">
+        <v>8</v>
+      </c>
+      <c r="L25" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>36</v>
+      </c>
+      <c r="B26" t="n">
+        <v>119</v>
+      </c>
+      <c r="C26" t="n">
+        <v>956</v>
+      </c>
+      <c r="D26" t="n">
+        <v>60</v>
+      </c>
+      <c r="E26" t="n">
+        <v>460</v>
+      </c>
+      <c r="F26" t="n">
+        <v>36</v>
+      </c>
+      <c r="G26" t="n">
+        <v>337</v>
+      </c>
+      <c r="H26" t="n">
+        <v>23</v>
+      </c>
+      <c r="I26" t="n">
+        <v>159</v>
+      </c>
+      <c r="J26" t="n">
+        <v>22</v>
+      </c>
+      <c r="K26" t="n">
+        <v>7</v>
+      </c>
+      <c r="L26" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>37</v>
+      </c>
+      <c r="B27" t="n">
+        <v>87</v>
+      </c>
+      <c r="C27" t="n">
+        <v>754</v>
+      </c>
+      <c r="D27" t="n">
+        <v>31</v>
+      </c>
+      <c r="E27" t="n">
+        <v>233</v>
+      </c>
+      <c r="F27" t="n">
+        <v>43</v>
+      </c>
+      <c r="G27" t="n">
+        <v>411</v>
+      </c>
+      <c r="H27" t="n">
+        <v>13</v>
+      </c>
+      <c r="I27" t="n">
+        <v>110</v>
+      </c>
+      <c r="J27" t="n">
+        <v>15</v>
+      </c>
+      <c r="K27" t="n">
+        <v>13</v>
+      </c>
+      <c r="L27" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>38</v>
+      </c>
+      <c r="B28" t="n">
+        <v>126</v>
+      </c>
+      <c r="C28" t="n">
+        <v>1088</v>
+      </c>
+      <c r="D28" t="n">
+        <v>56</v>
+      </c>
+      <c r="E28" t="n">
+        <v>483</v>
+      </c>
+      <c r="F28" t="n">
+        <v>49</v>
+      </c>
+      <c r="G28" t="n">
+        <v>426</v>
+      </c>
+      <c r="H28" t="n">
+        <v>21</v>
+      </c>
+      <c r="I28" t="n">
+        <v>179</v>
+      </c>
+      <c r="J28" t="n">
+        <v>19</v>
+      </c>
+      <c r="K28" t="n">
+        <v>5</v>
+      </c>
+      <c r="L28" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>39</v>
+      </c>
+      <c r="B29" t="n">
+        <v>134</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1111</v>
+      </c>
+      <c r="D29" t="n">
+        <v>59</v>
+      </c>
+      <c r="E29" t="n">
+        <v>428</v>
+      </c>
+      <c r="F29" t="n">
+        <v>59</v>
+      </c>
+      <c r="G29" t="n">
+        <v>547</v>
+      </c>
+      <c r="H29" t="n">
+        <v>16</v>
+      </c>
+      <c r="I29" t="n">
+        <v>136</v>
+      </c>
+      <c r="J29" t="n">
+        <v>26</v>
+      </c>
+      <c r="K29" t="n">
+        <v>24</v>
+      </c>
+      <c r="L29" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>40</v>
+      </c>
+      <c r="B30" t="n">
+        <v>121</v>
+      </c>
+      <c r="C30" t="n">
+        <v>956</v>
+      </c>
+      <c r="D30" t="n">
+        <v>45</v>
+      </c>
+      <c r="E30" t="n">
+        <v>304</v>
+      </c>
+      <c r="F30" t="n">
+        <v>53</v>
+      </c>
+      <c r="G30" t="n">
+        <v>441</v>
+      </c>
+      <c r="H30" t="n">
+        <v>23</v>
+      </c>
+      <c r="I30" t="n">
+        <v>211</v>
+      </c>
+      <c r="J30" t="n">
+        <v>18</v>
+      </c>
+      <c r="K30" t="n">
+        <v>20</v>
+      </c>
+      <c r="L30" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" t="n">
+        <v>118</v>
+      </c>
+      <c r="C31" t="n">
+        <v>900</v>
+      </c>
+      <c r="D31" t="n">
+        <v>61</v>
+      </c>
+      <c r="E31" t="n">
+        <v>461</v>
+      </c>
+      <c r="F31" t="n">
+        <v>38</v>
+      </c>
+      <c r="G31" t="n">
+        <v>330</v>
+      </c>
+      <c r="H31" t="n">
+        <v>19</v>
+      </c>
+      <c r="I31" t="n">
+        <v>109</v>
+      </c>
+      <c r="J31" t="n">
+        <v>30</v>
+      </c>
+      <c r="K31" t="n">
+        <v>7</v>
+      </c>
+      <c r="L31" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B32" t="n">
+        <v>117</v>
+      </c>
+      <c r="C32" t="n">
+        <v>1032</v>
+      </c>
+      <c r="D32" t="n">
+        <v>58</v>
+      </c>
+      <c r="E32" t="n">
+        <v>447</v>
+      </c>
+      <c r="F32" t="n">
+        <v>44</v>
+      </c>
+      <c r="G32" t="n">
+        <v>458</v>
+      </c>
+      <c r="H32" t="n">
+        <v>15</v>
+      </c>
+      <c r="I32" t="n">
+        <v>127</v>
+      </c>
+      <c r="J32" t="n">
+        <v>27</v>
+      </c>
+      <c r="K32" t="n">
+        <v>11</v>
+      </c>
+      <c r="L32" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" t="n">
+        <v>126</v>
+      </c>
+      <c r="C33" t="n">
+        <v>1043</v>
+      </c>
+      <c r="D33" t="n">
+        <v>63</v>
+      </c>
+      <c r="E33" t="n">
+        <v>491</v>
+      </c>
+      <c r="F33" t="n">
+        <v>47</v>
+      </c>
+      <c r="G33" t="n">
+        <v>426</v>
+      </c>
+      <c r="H33" t="n">
+        <v>16</v>
+      </c>
+      <c r="I33" t="n">
+        <v>126</v>
+      </c>
+      <c r="J33" t="n">
+        <v>28</v>
+      </c>
+      <c r="K33" t="n">
+        <v>18</v>
+      </c>
+      <c r="L33" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" t="n">
+        <v>3572</v>
+      </c>
+      <c r="C34" t="n">
+        <v>30311</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1654</v>
+      </c>
+      <c r="E34" t="n">
+        <v>12879</v>
+      </c>
+      <c r="F34" t="n">
+        <v>1393</v>
+      </c>
+      <c r="G34" t="n">
+        <v>13083</v>
+      </c>
+      <c r="H34" t="n">
+        <v>524</v>
+      </c>
+      <c r="I34" t="n">
+        <v>4334</v>
+      </c>
+      <c r="J34" t="n">
+        <v>706</v>
+      </c>
+      <c r="K34" t="n">
+        <v>334</v>
+      </c>
+      <c r="L34" t="n">
+        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -3097,7 +4404,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -4403,7 +5710,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -5638,16 +6945,16 @@
         <v>452</v>
       </c>
       <c r="F33" t="n">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G33" t="n">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="H33" t="n">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="I33" t="n">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="J33" t="n">
         <v>42</v>
@@ -5676,16 +6983,16 @@
         <v>12017</v>
       </c>
       <c r="F34" t="n">
-        <v>1206</v>
+        <v>1205</v>
       </c>
       <c r="G34" t="n">
-        <v>11604</v>
+        <v>11603</v>
       </c>
       <c r="H34" t="n">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="I34" t="n">
-        <v>4866</v>
+        <v>4867</v>
       </c>
       <c r="J34" t="n">
         <v>821</v>
@@ -5709,7 +7016,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -7015,7 +8322,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -8321,7 +9628,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -9627,7 +10934,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -10933,7 +12240,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -12048,10 +13355,10 @@
         <v>889</v>
       </c>
       <c r="D30" t="n">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E30" t="n">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="F30" t="n">
         <v>34</v>
@@ -12060,19 +13367,19 @@
         <v>345</v>
       </c>
       <c r="H30" t="n">
+        <v>21</v>
+      </c>
+      <c r="I30" t="n">
+        <v>151</v>
+      </c>
+      <c r="J30" t="n">
         <v>20</v>
-      </c>
-      <c r="I30" t="n">
-        <v>146</v>
-      </c>
-      <c r="J30" t="n">
-        <v>21</v>
       </c>
       <c r="K30" t="n">
         <v>7</v>
       </c>
       <c r="L30" t="n">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31">
@@ -12200,10 +13507,10 @@
         <v>30566</v>
       </c>
       <c r="D34" t="n">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="E34" t="n">
-        <v>13127</v>
+        <v>13122</v>
       </c>
       <c r="F34" t="n">
         <v>1314</v>
@@ -12212,19 +13519,19 @@
         <v>12682</v>
       </c>
       <c r="H34" t="n">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="I34" t="n">
-        <v>4757</v>
+        <v>4762</v>
       </c>
       <c r="J34" t="n">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="K34" t="n">
         <v>367</v>
       </c>
       <c r="L34" t="n">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -12239,7 +13546,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">

</xml_diff>